<commit_message>
Updated a Video in Excel file
</commit_message>
<xml_diff>
--- a/Documents/Docker-Videos.xlsx
+++ b/Documents/Docker-Videos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyCodes\Dockers\Docker-Crash-Course\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0BEFEB-8030-4DE9-A568-1CFBFD201558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F616218F-CC66-4C15-8CCC-23DC2AFB540D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E0F3D17A-EB6C-4033-BE3D-796241D7AB16}"/>
   </bookViews>
@@ -63,7 +63,7 @@
     <t>https://www.youtube.com/watch?v=Qw9zlE3t8Ko</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>https://www.youtube.com/watch?v=gAGEar5HQoU</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -491,7 +491,7 @@
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2"/>
@@ -515,6 +515,7 @@
     <hyperlink ref="A5" r:id="rId4" xr:uid="{1055894C-264C-4B6D-9E66-5F100E8CB80D}"/>
     <hyperlink ref="A6" r:id="rId5" xr:uid="{9E1BF69F-A154-413A-90F5-106CBFBBA83E}"/>
     <hyperlink ref="C3" r:id="rId6" xr:uid="{D67001B6-2773-4272-89AA-5409902C2CF4}"/>
+    <hyperlink ref="B5" r:id="rId7" xr:uid="{67F23ACC-AFFF-437A-A2D4-C285055130D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>